<commit_message>
Clean up files by removing custom styles
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_IND_CCS.xlsx
+++ b/SubRES_TMPL/SubRES_IND_CCS.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E116880-A44C-42ED-9FB2-2E965229FE53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38566C4-6CE6-4034-A3F4-0BA91C81C7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9D5618E0-D2A2-4912-B654-2E39BDAED497}"/>
   </bookViews>
@@ -521,30 +521,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -648,18 +633,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
@@ -692,152 +665,8 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Cambria"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -864,11 +693,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -877,169 +701,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
@@ -1055,7 +716,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1080,98 +741,6 @@
       </top>
       <bottom style="medium">
         <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1213,307 +782,123 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="7" borderId="1" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="38" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="55">
-    <cellStyle name="20% - Accent1 2" xfId="32" xr:uid="{61037AD9-0550-4C92-B6C5-E44963226FE4}"/>
-    <cellStyle name="20% - Accent2 2" xfId="36" xr:uid="{546719DC-A16F-41DF-B1A2-2618AA7621E3}"/>
-    <cellStyle name="20% - Accent3 2" xfId="40" xr:uid="{9B66B020-E167-433C-B3F9-B277B6CF2155}"/>
-    <cellStyle name="20% - Accent4 2" xfId="44" xr:uid="{47D8215F-5BB7-411D-8808-EEC4677F6707}"/>
-    <cellStyle name="20% - Accent5 2" xfId="48" xr:uid="{99913D4B-975B-472C-AE0B-DAC4B0FFE6DD}"/>
-    <cellStyle name="20% - Accent6 2" xfId="52" xr:uid="{8151DF33-5881-4F99-A089-2236810DEBE4}"/>
-    <cellStyle name="20% - Colore 2" xfId="9" xr:uid="{3E3DAF22-4D86-48A9-B6EE-8D230C1E993C}"/>
-    <cellStyle name="40% - Accent1 2" xfId="33" xr:uid="{453D62D2-079E-4CBB-9560-45E0F2B58DB2}"/>
-    <cellStyle name="40% - Accent2 2" xfId="37" xr:uid="{CE1C4268-9753-4A44-B417-C2544B1D86C1}"/>
-    <cellStyle name="40% - Accent3 2" xfId="41" xr:uid="{775BD512-2396-482C-9769-86B8D5520867}"/>
-    <cellStyle name="40% - Accent4 2" xfId="45" xr:uid="{680D3288-48E3-4E0F-9D87-C69D39DE3C22}"/>
-    <cellStyle name="40% - Accent5 2" xfId="49" xr:uid="{C25E6A8B-2470-412F-8A79-92B144E64B1F}"/>
-    <cellStyle name="40% - Accent6 2" xfId="53" xr:uid="{C9A9CE55-A594-4A33-892A-A72F616BC4AD}"/>
-    <cellStyle name="60% - Accent1 2" xfId="34" xr:uid="{6EDC8569-7E70-47D6-BB4D-920BC9D6637A}"/>
-    <cellStyle name="60% - Accent2 2" xfId="38" xr:uid="{B71BB7F1-5094-4D08-8EA3-4F034022526F}"/>
-    <cellStyle name="60% - Accent3 2" xfId="42" xr:uid="{AD92154D-D733-4CBF-AD91-0E5A73CFA6FD}"/>
-    <cellStyle name="60% - Accent4 2" xfId="46" xr:uid="{656C9227-2310-4DD3-A0D4-9021FAFCB5C6}"/>
-    <cellStyle name="60% - Accent5 2" xfId="50" xr:uid="{062D3DB1-CE82-4EAF-9BCA-C423FEC0CB00}"/>
-    <cellStyle name="60% - Accent6 2" xfId="54" xr:uid="{03FE49CB-EBD8-4DB8-BBF7-0560C15480AC}"/>
-    <cellStyle name="Accent2 2" xfId="35" xr:uid="{2684B6F3-388D-430C-B499-8DD1BF4C8306}"/>
-    <cellStyle name="Accent3 2" xfId="39" xr:uid="{B4F55954-8621-4B49-BAC6-880A56383608}"/>
-    <cellStyle name="Accent4 2" xfId="43" xr:uid="{9F9FD5D1-9641-47EB-AB0D-DEC13067AAC6}"/>
-    <cellStyle name="Accent5 2" xfId="47" xr:uid="{B4D1FB04-6BC8-4589-ACBA-318444142A7C}"/>
-    <cellStyle name="Accent6 2" xfId="51" xr:uid="{9BA19DF6-BA6F-4A35-9547-AF92C5375F99}"/>
-    <cellStyle name="Bad 2" xfId="22" xr:uid="{DE72CB1E-B9D5-42DC-9DC7-16A9E2A1B616}"/>
-    <cellStyle name="Calculation 2" xfId="26" xr:uid="{C97A4CB1-638D-40D5-AEB7-725C37B6E5DA}"/>
-    <cellStyle name="Check Cell 2" xfId="28" xr:uid="{059410AF-1EE2-48AB-A270-FC7D5218298C}"/>
-    <cellStyle name="Comma 2" xfId="10" xr:uid="{0ABA8B51-FCCD-40DB-958F-AE78849A8FFE}"/>
-    <cellStyle name="Explanatory Text 2" xfId="30" xr:uid="{B7DDFBA1-787A-4ABF-9958-36FF97AEED2E}"/>
-    <cellStyle name="Good 2" xfId="21" xr:uid="{D84817D1-D521-4BA1-A188-DD8674E41190}"/>
-    <cellStyle name="Heading 1 2" xfId="17" xr:uid="{E2F9BCE8-A94E-4BF5-BCE5-A2A96A0F2697}"/>
-    <cellStyle name="Heading 2 2" xfId="18" xr:uid="{0C6F311F-F8F6-4517-AE0C-6521A2648D51}"/>
-    <cellStyle name="Heading 3 2" xfId="19" xr:uid="{99CF5898-969B-473B-B9F3-6EA867CCBDC6}"/>
-    <cellStyle name="Heading 4 2" xfId="20" xr:uid="{B500383F-F56D-4B78-9038-005190613938}"/>
-    <cellStyle name="Input 2" xfId="24" xr:uid="{9DB7C141-2E66-401F-897B-5FDFEBD7B02C}"/>
-    <cellStyle name="Linked Cell 2" xfId="27" xr:uid="{83D152AA-77F1-45EC-BC95-01ED48426442}"/>
-    <cellStyle name="Neutral 2" xfId="23" xr:uid="{8F82BDDD-41DE-4B58-9EF1-9376CE4E4EF3}"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="3" xr:uid="{E1BCE1F9-C32B-49FB-A63B-D516C5E840D2}"/>
-    <cellStyle name="Normal 10 2" xfId="8" xr:uid="{403CABF5-5076-4EF0-B1C7-90DFA4621072}"/>
-    <cellStyle name="Normal 13" xfId="2" xr:uid="{7795B802-A17D-4590-A427-E52A73DAE426}"/>
-    <cellStyle name="Normal 15" xfId="5" xr:uid="{ECC42FCF-829B-4185-889D-06A7EB4A5E0F}"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{81BCDB32-370A-45D4-8768-8E71CE87AC81}"/>
-    <cellStyle name="Normal 3" xfId="14" xr:uid="{2E30EF23-A55F-4CD8-83E7-FFD4026CFADD}"/>
-    <cellStyle name="Normal 3 2" xfId="6" xr:uid="{5199F4FA-30A6-4F2B-B914-9F4ECA1F08E9}"/>
-    <cellStyle name="Normal 3 2 2" xfId="4" xr:uid="{AB77C6EE-5FAA-4EA6-92D0-2986F2803EAB}"/>
-    <cellStyle name="Normal 4" xfId="11" xr:uid="{C3AFA141-A2C0-4D00-BCC8-D2E525C207DA}"/>
-    <cellStyle name="Normal 4 2" xfId="7" xr:uid="{87BDABB2-3FF4-448F-8C91-A21FFDA39A5E}"/>
-    <cellStyle name="Normal 4 2 3 4" xfId="12" xr:uid="{49AF852B-ED69-4B51-AAC6-D5AE0788B9D3}"/>
-    <cellStyle name="Output 2" xfId="25" xr:uid="{D9531B1B-30DF-44CB-B4F6-D992B96429E1}"/>
-    <cellStyle name="Percent" xfId="13" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="15" xr:uid="{9BA5121B-5803-4DEA-AA6A-81217CE41DCB}"/>
-    <cellStyle name="Title 2" xfId="16" xr:uid="{0A17BEBA-7FC9-4A8B-B0B2-CD331F33AFE6}"/>
-    <cellStyle name="Total 2" xfId="31" xr:uid="{661F57BA-BA94-4744-8B69-F666AF67B8B3}"/>
-    <cellStyle name="Warning Text 2" xfId="29" xr:uid="{30DCA759-CD02-4D6B-8A03-297EE942C35E}"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -2168,7 +1553,7 @@
       <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="8" width="14.140625" style="6" customWidth="1"/>
@@ -2186,7 +1571,7 @@
     <col min="40" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2194,7 +1579,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2202,7 +1587,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -2210,7 +1595,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -2218,7 +1603,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2226,7 +1611,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -2234,7 +1619,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2242,7 +1627,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -2250,7 +1635,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -2258,7 +1643,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2266,7 +1651,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -2274,7 +1659,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -2282,7 +1667,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -2290,7 +1675,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -2298,7 +1683,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -2306,7 +1691,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2314,7 +1699,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:14" ht="102.75" customHeight="1">
+    <row r="17" spans="1:14" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="34" t="s">
         <v>61</v>
       </c>
@@ -2332,7 +1717,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14" ht="17.25" customHeight="1">
+    <row r="18" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -2340,7 +1725,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:14" ht="17.25" customHeight="1">
+    <row r="19" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -2356,7 +1741,7 @@
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
     </row>
-    <row r="20" spans="1:14" ht="17.25" customHeight="1">
+    <row r="20" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>0</v>
       </c>
@@ -2376,7 +1761,7 @@
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14" ht="17.25" customHeight="1">
+    <row r="21" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>13</v>
       </c>
@@ -2396,7 +1781,7 @@
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
     </row>
-    <row r="22" spans="1:14" ht="17.25" customHeight="1">
+    <row r="22" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
@@ -2406,7 +1791,7 @@
       <c r="E22" s="36"/>
       <c r="F22" s="36"/>
     </row>
-    <row r="23" spans="1:14" ht="17.25" customHeight="1">
+    <row r="23" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -2416,7 +1801,7 @@
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="1:14" ht="17.25" customHeight="1">
+    <row r="24" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -2428,7 +1813,7 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:14" ht="17.25" customHeight="1">
+    <row r="25" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="37"/>
       <c r="B25" s="37"/>
       <c r="C25" s="37"/>
@@ -2438,7 +1823,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:14" ht="17.25" customHeight="1">
+    <row r="26" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="33"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
@@ -2446,7 +1831,7 @@
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -2454,7 +1839,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -2462,7 +1847,7 @@
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2470,7 +1855,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2478,7 +1863,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2486,7 +1871,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2494,7 +1879,7 @@
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2502,7 +1887,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2510,7 +1895,7 @@
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2518,7 +1903,7 @@
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2526,7 +1911,7 @@
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2534,7 +1919,7 @@
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -2542,7 +1927,7 @@
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -2550,7 +1935,7 @@
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -2558,7 +1943,7 @@
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -2566,7 +1951,7 @@
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -2574,7 +1959,7 @@
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -2582,7 +1967,7 @@
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2607,13 +1992,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E65932-8AD8-48FB-989E-7D3601E44567}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.7109375" style="16" bestFit="1" customWidth="1"/>
@@ -2634,7 +2020,7 @@
     <col min="21" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -2659,7 +2045,7 @@
       <c r="S3" s="20"/>
       <c r="T3" s="20"/>
     </row>
-    <row r="4" spans="1:20" ht="30.75" thickBot="1">
+    <row r="4" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2718,7 +2104,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="51">
+    <row r="5" spans="1:20" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="28" t="s">
         <v>63</v>
       </c>
@@ -2775,7 +2161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>36</v>
       </c>
@@ -2806,7 +2192,7 @@
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="str">
         <f>N7</f>
         <v>I-DMD-ONM-N1</v>
@@ -2862,7 +2248,7 @@
       <c r="S7" s="32"/>
       <c r="T7" s="32"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C8" s="16" t="s">
         <v>41</v>
       </c>
@@ -2873,7 +2259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C9" s="16" t="s">
         <v>42</v>
       </c>
@@ -2884,7 +2270,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C10" s="16" t="s">
         <v>43</v>
       </c>
@@ -2895,7 +2281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C11" s="16" t="s">
         <v>44</v>
       </c>
@@ -2906,7 +2292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C12" s="16" t="s">
         <v>45</v>
       </c>
@@ -2917,7 +2303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C13" s="16" t="s">
         <v>46</v>
       </c>
@@ -2928,7 +2314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C14" s="16" t="s">
         <v>47</v>
       </c>
@@ -2939,7 +2325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="C15" s="16" t="s">
         <v>48</v>
       </c>
@@ -2950,7 +2336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30" t="s">
@@ -2969,12 +2355,12 @@
       </c>
       <c r="K16" s="30"/>
     </row>
-    <row r="22" spans="9:11">
+    <row r="22" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I22" s="23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="9:11">
+    <row r="23" spans="9:11" x14ac:dyDescent="0.2">
       <c r="I23" s="24" t="s">
         <v>59</v>
       </c>

</xml_diff>